<commit_message>
vinhndq update upload de thi
</commit_message>
<xml_diff>
--- a/public/assets/media/excel/excel_download.xlsx
+++ b/public/assets/media/excel/excel_download.xlsx
@@ -1,28 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\duan-poly\api-student-capacity\public\assets\media\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Quang Vinh\Workspace\fpoly\student-capacity-2\api-student-capacity\public\assets\media\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461B4C96-3B01-4647-9CDB-340BABD85F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4373EE99-9F9D-4938-BBE1-8808432C6B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Câu hỏi" sheetId="1" r:id="rId1"/>
+    <sheet name="Ảnh" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" forceFullCalc="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -117,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -131,21 +135,9 @@
     <t>Đáp án đúng</t>
   </si>
   <si>
-    <t>Con gà</t>
-  </si>
-  <si>
-    <t>Con mèo</t>
-  </si>
-  <si>
     <t>Cá xấu</t>
   </si>
   <si>
-    <t>Con voi</t>
-  </si>
-  <si>
-    <t>Con ngựa</t>
-  </si>
-  <si>
     <t>Đại bảng</t>
   </si>
   <si>
@@ -155,9 +147,6 @@
     <t>Giun</t>
   </si>
   <si>
-    <t>Cá voi</t>
-  </si>
-  <si>
     <t>Một đáp án</t>
   </si>
   <si>
@@ -170,29 +159,50 @@
     <t>Trung bình</t>
   </si>
   <si>
-    <t>Câu hỏi by excel 8</t>
-  </si>
-  <si>
     <t>Câu hỏi by excel 9</t>
   </si>
   <si>
     <t>Câu hỏi by excel 10</t>
   </si>
   <si>
-    <t>Đại bàng</t>
-  </si>
-  <si>
     <t>Thể loại câu hỏi</t>
   </si>
   <si>
     <t xml:space="preserve">Mức độ </t>
+  </si>
+  <si>
+    <t>Mã ảnh</t>
+  </si>
+  <si>
+    <t>Ảnh</t>
+  </si>
+  <si>
+    <t>anh1</t>
+  </si>
+  <si>
+    <t>anh2</t>
+  </si>
+  <si>
+    <t>Câu hỏi by [anh1] Quang Vinh</t>
+  </si>
+  <si>
+    <t>[anh2]</t>
+  </si>
+  <si>
+    <t>Khủng long</t>
+  </si>
+  <si>
+    <t>Rồng</t>
+  </si>
+  <si>
+    <t>Heo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -243,6 +253,12 @@
       <sz val="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -265,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -274,6 +290,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -292,6 +311,111 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1684020</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>487680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E60A2C59-5F1B-D73E-084E-6FA44AC0CA80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1607820" y="300990"/>
+          <a:ext cx="1684020" cy="453390"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1684020</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>487680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F90D821-F067-45E2-9AC7-724BD97217FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1607820" y="300990"/>
+          <a:ext cx="1684020" cy="453390"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -582,31 +706,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="255.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -618,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -627,122 +751,109 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="C12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="C15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="10:10">
-      <c r="J18" s="1" t="s">
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J17" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="10:10">
-      <c r="J20" s="1" t="s">
+    <row r="19" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J19" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -751,22 +862,63 @@
   <dataConsolidate/>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A18" xr:uid="{85164911-4EAC-4943-AE71-BF27AD6FF322}">
-      <formula1>"Một đáp án,Nhiều đáp án"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D198" xr:uid="{9F3D142E-7F65-4A9F-B137-6914540F61D4}">
-      <formula1>"Đáp án đúng"</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9" xr:uid="{31D8A5D7-9C36-4321-B653-A27B6A74B5EA}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8" xr:uid="{31D8A5D7-9C36-4321-B653-A27B6A74B5EA}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:F53 E2:E17" xr:uid="{9BCE8E96-6CC0-4B3B-B787-63D68448C58D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:F52 E2:E16" xr:uid="{9BCE8E96-6CC0-4B3B-B787-63D68448C58D}">
       <formula1>"Dễ,Trung bình,Khó"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D197" xr:uid="{9F3D142E-7F65-4A9F-B137-6914540F61D4}">
+      <formula1>"Đáp án đúng"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A17" xr:uid="{85164911-4EAC-4943-AE71-BF27AD6FF322}">
+      <formula1>"Một đáp án,Nhiều đáp án"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB016F8F-04E8-45CE-9B6A-DCCDB0F4D946}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
vinhndq update upload đề thi - sửa file excel mẫu và lưu ảnh với aws cloud
</commit_message>
<xml_diff>
--- a/public/assets/media/excel/excel_download.xlsx
+++ b/public/assets/media/excel/excel_download.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Quang Vinh\Workspace\fpoly\student-capacity-2\api-student-capacity\public\assets\media\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4373EE99-9F9D-4938-BBE1-8808432C6B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02826AB2-6402-4744-8945-4B67A9AF245A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Câu hỏi" sheetId="1" r:id="rId1"/>
     <sheet name="Ảnh" sheetId="3" r:id="rId2"/>
+    <sheet name="Hướng dẫn" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" forceFullCalc="1"/>
   <extLst>
@@ -121,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -135,36 +136,15 @@
     <t>Đáp án đúng</t>
   </si>
   <si>
-    <t>Cá xấu</t>
-  </si>
-  <si>
-    <t>Đại bảng</t>
-  </si>
-  <si>
-    <t>Voi</t>
-  </si>
-  <si>
-    <t>Giun</t>
-  </si>
-  <si>
     <t>Một đáp án</t>
   </si>
   <si>
-    <t>Nhiều đáp án</t>
-  </si>
-  <si>
     <t>Dễ</t>
   </si>
   <si>
     <t>Trung bình</t>
   </si>
   <si>
-    <t>Câu hỏi by excel 9</t>
-  </si>
-  <si>
-    <t>Câu hỏi by excel 10</t>
-  </si>
-  <si>
     <t>Thể loại câu hỏi</t>
   </si>
   <si>
@@ -183,26 +163,83 @@
     <t>anh2</t>
   </si>
   <si>
-    <t>Câu hỏi by [anh1] Quang Vinh</t>
-  </si>
-  <si>
-    <t>[anh2]</t>
-  </si>
-  <si>
-    <t>Khủng long</t>
-  </si>
-  <si>
-    <t>Rồng</t>
-  </si>
-  <si>
-    <t>Heo</t>
+    <t>Copy công thức từ file word và dán vào file excel</t>
+  </si>
+  <si>
+    <t>Trong file excel, click đúp chuột vào công thức vừa copy, nếu như hiện ra cửa sổ như sau thì chọn "Ok"</t>
+  </si>
+  <si>
+    <t>Click lại vào công thức sau khi đã convert và tiến hành copy công thức với tổ hợp phím "Ctrl + C"</t>
+  </si>
+  <si>
+    <t>Dán công thức vừa copy vào câu hỏi/đáp án chứa công thức</t>
+  </si>
+  <si>
+    <t>Để thêm ảnh, trong câu hỏi/đáp án có chứa ảnh, hãy điền mã ảnh theo cú pháp [anh*] với * là số tự nhiên, mã ảnh không được trùng nhau</t>
+  </si>
+  <si>
+    <t>Trong sheet "Ảnh", điền mã ảnh (bỏ cặp dấu []) và ảnh tương ứng với mã ảnh phía sheet "Câu hỏi"</t>
+  </si>
+  <si>
+    <t>Cho hàm số 𝑦=𝑓(𝑥) có bảng biến thiên như sau: [anh1] Hàm số 𝑦=𝑓(𝑥) đồng biến trên khoảng nào sau đây?</t>
+  </si>
+  <si>
+    <t>(-∞;0)</t>
+  </si>
+  <si>
+    <t>(-2;0)</t>
+  </si>
+  <si>
+    <t>(0;+∞)</t>
+  </si>
+  <si>
+    <t>(-4;+∞)</t>
+  </si>
+  <si>
+    <t>Cho hàm số 𝑦=𝑓(𝑥) có đồ thị như hình vẽ bên dưới. Hàm số 𝑦=𝑓(𝑥) nghịch biến trên khoảng nào dưới đây? [anh2]</t>
+  </si>
+  <si>
+    <t>(-1;0)</t>
+  </si>
+  <si>
+    <t>(0;1)</t>
+  </si>
+  <si>
+    <t>(0;2)</t>
+  </si>
+  <si>
+    <t>(1;+∞)</t>
+  </si>
+  <si>
+    <t>Cho hàm số 𝑦=𝑓(𝑥) có bảng biến thiên như sau:[anh3] Hàm số 𝑦=𝑓(𝑥) có giá trị cực đại là</t>
+  </si>
+  <si>
+    <t>x=-3</t>
+  </si>
+  <si>
+    <t>y=-4</t>
+  </si>
+  <si>
+    <t>x=0</t>
+  </si>
+  <si>
+    <t>y=-3</t>
+  </si>
+  <si>
+    <t>Hàm số 𝑦=𝑓(𝑥) liên tục trên R và có đồ thị như hình vẽ bên dưới: [anh4] Số điểm cực tiểu của hàm số 𝑦=𝑓(𝑥) là</t>
+  </si>
+  <si>
+    <t>anh3</t>
+  </si>
+  <si>
+    <t>anh4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -259,6 +296,24 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -281,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -292,8 +347,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -315,25 +380,25 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1684020</xdr:colOff>
+      <xdr:colOff>1706880</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>487680</xdr:rowOff>
+      <xdr:rowOff>458888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="2" name="Picture 1" descr="Diagram&#10;&#10;Description automatically generated">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E60A2C59-5F1B-D73E-084E-6FA44AC0CA80}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F7DF890-200C-2645-A634-BCDFA3897CDB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -342,21 +407,196 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1607820" y="300990"/>
-          <a:ext cx="1684020" cy="453390"/>
+          <a:off x="1607820" y="266700"/>
+          <a:ext cx="1706880" cy="458888"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1054848</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1165860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12EC0797-7340-6D55-7589-9906D4F1D9FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1607820" y="1005840"/>
+          <a:ext cx="1054848" cy="1165860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1823328</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>449580</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="A picture containing diagram&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9D425B1-56AB-7565-FB77-8239BD8B971D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1607820" y="2194560"/>
+          <a:ext cx="1823328" cy="449580"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1219199</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1063374</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Diagram&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40D44982-FC01-CEF4-C44D-1826E71DCA3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1607820" y="2933700"/>
+          <a:ext cx="1219199" cy="1063374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3383281</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{728119A8-4E60-4DB0-BF89-A8F020766BEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5173980" y="15240"/>
+          <a:ext cx="3383281" cy="1173480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -369,21 +609,21 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1684020</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>487680</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F90D821-F067-45E2-9AC7-724BD97217FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{513D04D8-4610-B30F-32FF-783AD08B7260}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -392,21 +632,190 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1607820" y="300990"/>
-          <a:ext cx="1684020" cy="453390"/>
+          <a:off x="6248400" y="1226821"/>
+          <a:ext cx="3131820" cy="1158239"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>144779</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3287</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A1D3BC8-491C-7A48-B80E-B6C2D720FE38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6248400" y="2385060"/>
+          <a:ext cx="3230879" cy="811007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>11393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3078480</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1005840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C28F4579-2DDC-CA33-33E6-F9A678947058}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:srcRect l="14601" r="41687"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6393180" y="3204173"/>
+          <a:ext cx="3078480" cy="994447"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7879079</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1089660</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3337560</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1031846</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A0BC1E3-332D-E4D8-C04C-0B6D8FE02D1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7879079" y="4777740"/>
+          <a:ext cx="3337561" cy="1039466"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1036320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{232BC40F-5CB7-65B1-E330-74F37903BCDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6393180" y="5311141"/>
+          <a:ext cx="3093720" cy="1036319"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -708,14 +1117,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -730,7 +1139,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -742,7 +1151,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -751,108 +1160,143 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3"/>
+      <c r="C3" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="8" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C5" s="3" t="s">
+    <row r="5" spans="1:11" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C9" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
+    </row>
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="6"/>
+      <c r="C11" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C12" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="14" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="6"/>
+      <c r="C15" s="7">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C13" s="1" t="s">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C17" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J17" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="10:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
       <c r="J19" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,7 +1310,7 @@
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:F52 E2:E16" xr:uid="{9BCE8E96-6CC0-4B3B-B787-63D68448C58D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:F52 E2:E17" xr:uid="{9BCE8E96-6CC0-4B3B-B787-63D68448C58D}">
       <formula1>"Dễ,Trung bình,Khó"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D197" xr:uid="{9F3D142E-7F65-4A9F-B137-6914540F61D4}">
@@ -886,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB016F8F-04E8-45CE-9B6A-DCCDB0F4D946}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,27 +1342,86 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="6" spans="1:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239FFF5C-FA55-4CBB-AEA9-BA36B8CB9915}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="93.21875" customWidth="1"/>
+    <col min="2" max="2" width="45" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>